<commit_message>
brute force algorithm initialized
</commit_message>
<xml_diff>
--- a/Adatok.xlsx
+++ b/Adatok.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agnes\Desktop\orarend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01840128-0A6E-497D-99CF-D1C52294322D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7CEBF5-09F3-48C6-8DE8-1DFBF0956C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{11A5BB39-AF8D-4C14-AEFC-0737B200F124}"/>
+    <workbookView xWindow="6000" yWindow="0" windowWidth="18000" windowHeight="9360" xr2:uid="{11A5BB39-AF8D-4C14-AEFC-0737B200F124}"/>
   </bookViews>
   <sheets>
     <sheet name="Tanarok" sheetId="1" r:id="rId1"/>
@@ -37,13 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
-  <si>
-    <t>Kerekes</t>
-  </si>
-  <si>
-    <t>Tolmacsi</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Nagy</t>
   </si>
@@ -51,36 +45,15 @@
     <t>Kis</t>
   </si>
   <si>
-    <t>Janos</t>
-  </si>
-  <si>
-    <t>Agnes</t>
-  </si>
-  <si>
     <t>Jozsef</t>
   </si>
   <si>
     <t>Balint</t>
   </si>
   <si>
-    <t>H1, K3, SZ5</t>
-  </si>
-  <si>
-    <t>H2, K4, P6</t>
-  </si>
-  <si>
-    <t>K5, SZ7, CS2, P1</t>
-  </si>
-  <si>
-    <t>H1, H2, H3, K1, K2, K3</t>
-  </si>
-  <si>
     <t>1,2,3,4,5,6,7,8</t>
   </si>
   <si>
-    <t>1,2,3,4</t>
-  </si>
-  <si>
     <t>1,2,3,4,5,6,7,8,9,10,11,12</t>
   </si>
   <si>
@@ -103,6 +76,24 @@
   </si>
   <si>
     <t>Luca</t>
+  </si>
+  <si>
+    <t>K5</t>
+  </si>
+  <si>
+    <t>SZ7</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>K5,SZ7,CS2,P1</t>
+  </si>
+  <si>
+    <t>H1,H2,H3,K1,K2,K3</t>
   </si>
 </sst>
 </file>
@@ -475,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC14E19B-D511-4375-89F0-DE3C02CCBC01}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,16 +483,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -509,49 +500,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
       <c r="E2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
         <v>1</v>
       </c>
     </row>
@@ -564,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E95653-3951-4A98-B902-EBA017CE50B3}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,13 +532,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1">
         <v>6</v>
@@ -592,13 +549,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -609,13 +566,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -626,13 +583,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>11</v>

</xml_diff>